<commit_message>
update data corrections file
Update data correctiosn file and add the .rda sent by Pablo to accomplish corrections for NSS
</commit_message>
<xml_diff>
--- a/build/nss 2020/Data_Corrections_NS2020.xlsx
+++ b/build/nss 2020/Data_Corrections_NS2020.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7485"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7485" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Set Card" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,9 @@
     <sheet name="Bio" sheetId="3" r:id="rId3"/>
     <sheet name="Bryozoan Dataset 2020" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Set Card'!$A$1:$K$41</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -199,7 +202,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="75">
   <si>
     <t>Species</t>
   </si>
@@ -390,15 +393,6 @@
     <t>Nor Likely. NA or Remove</t>
   </si>
   <si>
-    <t>I would guess 10</t>
-  </si>
-  <si>
-    <t>I would guess 13</t>
-  </si>
-  <si>
-    <t>??</t>
-  </si>
-  <si>
     <t>good</t>
   </si>
   <si>
@@ -418,6 +412,21 @@
   </si>
   <si>
     <t>Five level (0-4) parameter was added at set 30 to reflect percent byozoan coverage on lobster carapace. Coding was misused for this set(31)  and we need to substract one from each value.</t>
+  </si>
+  <si>
+    <t>leave NA</t>
+  </si>
+  <si>
+    <t>Pabs format1</t>
+  </si>
+  <si>
+    <t>Pabs format2</t>
+  </si>
+  <si>
+    <t>1:16:00 PM</t>
+  </si>
+  <si>
+    <t>11:37:00 AM</t>
   </si>
 </sst>
 </file>
@@ -460,7 +469,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -483,6 +492,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -498,13 +513,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="21" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="21" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -513,6 +527,10 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="2" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="21" fontId="1" fillId="2" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -795,10 +813,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M41"/>
+  <dimension ref="A1:O41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D39" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="N61" sqref="N61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -808,9 +826,12 @@
     <col min="8" max="8" width="14.7109375" customWidth="1"/>
     <col min="9" max="9" width="18.85546875" customWidth="1"/>
     <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="53.7109375" customWidth="1"/>
+    <col min="14" max="14" width="65" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="61.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -844,8 +865,14 @@
       <c r="K1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N1" t="s">
+        <v>71</v>
+      </c>
+      <c r="O1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2020</v>
       </c>
@@ -877,11 +904,19 @@
         <v>31</v>
       </c>
       <c r="M2" t="str">
-        <f>"y$set$"&amp;G2&amp;"[y$set$set.number == "&amp;C2&amp;"] &lt;- "&amp;I2</f>
+        <f>"y$set$"&amp;$G2&amp;"[y$set$set.number == "&amp;$C2&amp;"] &lt;- "&amp;$I2</f>
         <v>y$set$longitude.stop[y$set$set.number == 1] &lt;- 6426.14</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N2" t="str">
+        <f>"index = y$set$set.number == "&amp;$C2&amp;" PAR "&amp;"y$set$"&amp;$G2&amp;"[index] &lt;- "&amp;$I2</f>
+        <v>index = y$set$set.number == 1 PAR y$set$longitude.stop[index] &lt;- 6426.14</v>
+      </c>
+      <c r="O2" t="str">
+        <f>"y$set$"&amp;$G2&amp;"[index] &lt;- "&amp;$I2</f>
+        <v>y$set$longitude.stop[index] &lt;- 6426.14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2020</v>
       </c>
@@ -913,11 +948,19 @@
         <v>11</v>
       </c>
       <c r="M3" t="str">
-        <f>"y$set$"&amp;G3&amp;"[y$set$set.number == "&amp;C3&amp;"] &lt;- "&amp;I3</f>
+        <f t="shared" ref="M3:M39" si="0">"y$set$"&amp;$G3&amp;"[y$set$set.number == "&amp;$C3&amp;"] &lt;- "&amp;$I3</f>
         <v>y$set$latitude.stop[y$set$set.number == 9] &lt;- 4638.53</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N3" t="str">
+        <f t="shared" ref="N3:N41" si="1">"index = y$set$set.number == "&amp;$C3&amp;" PAR "&amp;"y$set$"&amp;$G3&amp;"[index] &lt;- "&amp;$I3</f>
+        <v>index = y$set$set.number == 9 PAR y$set$latitude.stop[index] &lt;- 4638.53</v>
+      </c>
+      <c r="O3" t="str">
+        <f t="shared" ref="O3:O41" si="2">"y$set$"&amp;$G3&amp;"[index] &lt;- "&amp;$I3</f>
+        <v>y$set$latitude.stop[index] &lt;- 4638.53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2020</v>
       </c>
@@ -949,11 +992,19 @@
         <v>30</v>
       </c>
       <c r="M4" t="str">
-        <f>"y$set$"&amp;G4&amp;"[y$set$set.number == "&amp;C4&amp;"] &lt;- "&amp;I4</f>
+        <f t="shared" si="0"/>
         <v>y$set$latitude.start[y$set$set.number == 10] &lt;- 4644</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N4" t="str">
+        <f t="shared" si="1"/>
+        <v>index = y$set$set.number == 10 PAR y$set$latitude.start[index] &lt;- 4644</v>
+      </c>
+      <c r="O4" t="str">
+        <f t="shared" si="2"/>
+        <v>y$set$latitude.start[index] &lt;- 4644</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2020</v>
       </c>
@@ -985,11 +1036,19 @@
         <v>31</v>
       </c>
       <c r="M5" t="str">
-        <f>"y$set$"&amp;G5&amp;"[y$set$set.number == "&amp;C5&amp;"] &lt;- "&amp;I5</f>
+        <f t="shared" si="0"/>
         <v>y$set$experiment[y$set$set.number == 10] &lt;- 1</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N5" t="str">
+        <f t="shared" si="1"/>
+        <v>index = y$set$set.number == 10 PAR y$set$experiment[index] &lt;- 1</v>
+      </c>
+      <c r="O5" t="str">
+        <f t="shared" si="2"/>
+        <v>y$set$experiment[index] &lt;- 1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2020</v>
       </c>
@@ -1021,11 +1080,19 @@
         <v>31</v>
       </c>
       <c r="M6" t="str">
-        <f>"y$set$"&amp;G6&amp;"[y$set$set.number == "&amp;C6&amp;"] &lt;- "&amp;I6</f>
+        <f t="shared" si="0"/>
         <v>y$set$longitude.stop[y$set$set.number == 12] &lt;- 6426.3</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N6" t="str">
+        <f t="shared" si="1"/>
+        <v>index = y$set$set.number == 12 PAR y$set$longitude.stop[index] &lt;- 6426.3</v>
+      </c>
+      <c r="O6" t="str">
+        <f t="shared" si="2"/>
+        <v>y$set$longitude.stop[index] &lt;- 6426.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2020</v>
       </c>
@@ -1057,11 +1124,19 @@
         <v>31</v>
       </c>
       <c r="M7" t="str">
-        <f>"y$set$"&amp;G7&amp;"[y$set$set.number == "&amp;C7&amp;"] &lt;- "&amp;I7</f>
+        <f t="shared" si="0"/>
         <v>y$set$current[y$set$set.number == 18] &lt;- 1</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N7" t="str">
+        <f t="shared" si="1"/>
+        <v>index = y$set$set.number == 18 PAR y$set$current[index] &lt;- 1</v>
+      </c>
+      <c r="O7" t="str">
+        <f t="shared" si="2"/>
+        <v>y$set$current[index] &lt;- 1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2020</v>
       </c>
@@ -1086,18 +1161,26 @@
       <c r="H8" s="3">
         <v>0.55069444444444449</v>
       </c>
-      <c r="I8" s="5">
-        <v>0.55277777777777781</v>
+      <c r="I8" s="16" t="s">
+        <v>73</v>
       </c>
       <c r="J8" t="s">
         <v>31</v>
       </c>
       <c r="M8" t="str">
-        <f>"y$set$"&amp;G8&amp;"[y$set$set.number == "&amp;C8&amp;"] &lt;- "&amp;TEXT(I8,"hh:mm:ss")</f>
-        <v>y$set$stop.time[y$set$set.number == 23] &lt;- 13:16:00</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>y$set$stop.time[y$set$set.number == 23] &lt;- 1:16:00 PM</v>
+      </c>
+      <c r="N8" t="str">
+        <f t="shared" si="1"/>
+        <v>index = y$set$set.number == 23 PAR y$set$stop.time[index] &lt;- 1:16:00 PM</v>
+      </c>
+      <c r="O8" t="str">
+        <f t="shared" si="2"/>
+        <v>y$set$stop.time[index] &lt;- 1:16:00 PM</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2020</v>
       </c>
@@ -1129,11 +1212,19 @@
         <v>11</v>
       </c>
       <c r="M9" t="str">
-        <f>"y$set$"&amp;G9&amp;"[y$set$set.number == "&amp;C9&amp;"] &lt;- "&amp;I9</f>
+        <f t="shared" si="0"/>
         <v>y$set$latitude.stop[y$set$set.number == 23] &lt;- 4643.3</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N9" t="str">
+        <f t="shared" si="1"/>
+        <v>index = y$set$set.number == 23 PAR y$set$latitude.stop[index] &lt;- 4643.3</v>
+      </c>
+      <c r="O9" t="str">
+        <f t="shared" si="2"/>
+        <v>y$set$latitude.stop[index] &lt;- 4643.3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2020</v>
       </c>
@@ -1165,11 +1256,19 @@
         <v>33</v>
       </c>
       <c r="M10" t="str">
-        <f>"y$set$"&amp;G10&amp;"[y$set$set.number == "&amp;C10&amp;"] &lt;- "&amp;I10</f>
+        <f t="shared" si="0"/>
         <v>y$set$longitude.stop[y$set$set.number == 23] &lt;- 6436.96</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N10" t="str">
+        <f t="shared" si="1"/>
+        <v>index = y$set$set.number == 23 PAR y$set$longitude.stop[index] &lt;- 6436.96</v>
+      </c>
+      <c r="O10" t="str">
+        <f t="shared" si="2"/>
+        <v>y$set$longitude.stop[index] &lt;- 6436.96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2020</v>
       </c>
@@ -1201,11 +1300,19 @@
         <v>30</v>
       </c>
       <c r="M11" t="str">
-        <f>"y$set$"&amp;G11&amp;"[y$set$set.number == "&amp;C11&amp;"] &lt;- "&amp;I11</f>
+        <f t="shared" si="0"/>
         <v>y$set$latitude.stop[y$set$set.number == 24] &lt;- 4648.52</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N11" t="str">
+        <f t="shared" si="1"/>
+        <v>index = y$set$set.number == 24 PAR y$set$latitude.stop[index] &lt;- 4648.52</v>
+      </c>
+      <c r="O11" t="str">
+        <f t="shared" si="2"/>
+        <v>y$set$latitude.stop[index] &lt;- 4648.52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2020</v>
       </c>
@@ -1237,11 +1344,19 @@
         <v>34</v>
       </c>
       <c r="M12" t="str">
-        <f>"y$set$"&amp;G12&amp;"[y$set$set.number == "&amp;C12&amp;"] &lt;- "&amp;I12</f>
+        <f t="shared" si="0"/>
         <v>y$set$wind.force[y$set$set.number == 27] &lt;- 3</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N12" t="str">
+        <f t="shared" si="1"/>
+        <v>index = y$set$set.number == 27 PAR y$set$wind.force[index] &lt;- 3</v>
+      </c>
+      <c r="O12" t="str">
+        <f t="shared" si="2"/>
+        <v>y$set$wind.force[index] &lt;- 3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2020</v>
       </c>
@@ -1273,11 +1388,19 @@
         <v>33</v>
       </c>
       <c r="M13" t="str">
-        <f>"y$set$"&amp;G13&amp;"[y$set$set.number == "&amp;C13&amp;"] &lt;- "&amp;I13</f>
+        <f t="shared" si="0"/>
         <v>y$set$longitude.start[y$set$set.number == 31] &lt;- 6355.55</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N13" t="str">
+        <f t="shared" si="1"/>
+        <v>index = y$set$set.number == 31 PAR y$set$longitude.start[index] &lt;- 6355.55</v>
+      </c>
+      <c r="O13" t="str">
+        <f t="shared" si="2"/>
+        <v>y$set$longitude.start[index] &lt;- 6355.55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2020</v>
       </c>
@@ -1309,11 +1432,19 @@
         <v>33</v>
       </c>
       <c r="M14" t="str">
-        <f>"y$set$"&amp;G14&amp;"[y$set$set.number == "&amp;C14&amp;"] &lt;- "&amp;I14</f>
+        <f t="shared" si="0"/>
         <v>y$set$longitude.stop[y$set$set.number == 31] &lt;- 6354.95</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N14" t="str">
+        <f t="shared" si="1"/>
+        <v>index = y$set$set.number == 31 PAR y$set$longitude.stop[index] &lt;- 6354.95</v>
+      </c>
+      <c r="O14" t="str">
+        <f t="shared" si="2"/>
+        <v>y$set$longitude.stop[index] &lt;- 6354.95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2020</v>
       </c>
@@ -1345,11 +1476,19 @@
         <v>30</v>
       </c>
       <c r="M15" t="str">
-        <f>"y$set$"&amp;G15&amp;"[y$set$set.number == "&amp;C15&amp;"] &lt;- "&amp;I15</f>
+        <f t="shared" si="0"/>
         <v>y$set$depth.end[y$set$set.number == 33] &lt;- 10</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N15" t="str">
+        <f t="shared" si="1"/>
+        <v>index = y$set$set.number == 33 PAR y$set$depth.end[index] &lt;- 10</v>
+      </c>
+      <c r="O15" t="str">
+        <f t="shared" si="2"/>
+        <v>y$set$depth.end[index] &lt;- 10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2020</v>
       </c>
@@ -1381,11 +1520,19 @@
         <v>31</v>
       </c>
       <c r="M16" t="str">
-        <f>"y$set$"&amp;G16&amp;"[y$set$set.number == "&amp;C16&amp;"] &lt;- "&amp;I16</f>
+        <f t="shared" si="0"/>
         <v>y$set$experiment[y$set$set.number == 34] &lt;- 1</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N16" t="str">
+        <f t="shared" si="1"/>
+        <v>index = y$set$set.number == 34 PAR y$set$experiment[index] &lt;- 1</v>
+      </c>
+      <c r="O16" t="str">
+        <f t="shared" si="2"/>
+        <v>y$set$experiment[index] &lt;- 1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2020</v>
       </c>
@@ -1417,11 +1564,19 @@
         <v>31</v>
       </c>
       <c r="M17" t="str">
-        <f>"y$set$"&amp;G17&amp;"[y$set$set.number == "&amp;C17&amp;"] &lt;- "&amp;I17</f>
+        <f t="shared" si="0"/>
         <v>y$set$latitude.start[y$set$set.number == 35] &lt;- 4646.05</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N17" t="str">
+        <f t="shared" si="1"/>
+        <v>index = y$set$set.number == 35 PAR y$set$latitude.start[index] &lt;- 4646.05</v>
+      </c>
+      <c r="O17" t="str">
+        <f t="shared" si="2"/>
+        <v>y$set$latitude.start[index] &lt;- 4646.05</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2020</v>
       </c>
@@ -1453,11 +1608,19 @@
         <v>31</v>
       </c>
       <c r="M18" t="str">
-        <f>"y$set$"&amp;G18&amp;"[y$set$set.number == "&amp;C18&amp;"] &lt;- "&amp;I18</f>
+        <f t="shared" si="0"/>
         <v>y$set$wind.force[y$set$set.number == 35] &lt;- 3</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N18" t="str">
+        <f t="shared" si="1"/>
+        <v>index = y$set$set.number == 35 PAR y$set$wind.force[index] &lt;- 3</v>
+      </c>
+      <c r="O18" t="str">
+        <f t="shared" si="2"/>
+        <v>y$set$wind.force[index] &lt;- 3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2020</v>
       </c>
@@ -1489,11 +1652,19 @@
         <v>31</v>
       </c>
       <c r="M19" t="str">
-        <f>"y$set$"&amp;G19&amp;"[y$set$set.number == "&amp;C19&amp;"] &lt;- "&amp;I19</f>
+        <f t="shared" si="0"/>
         <v>y$set$longitude.stop[y$set$set.number == 37] &lt;- 6446.18</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N19" t="str">
+        <f t="shared" si="1"/>
+        <v>index = y$set$set.number == 37 PAR y$set$longitude.stop[index] &lt;- 6446.18</v>
+      </c>
+      <c r="O19" t="str">
+        <f t="shared" si="2"/>
+        <v>y$set$longitude.stop[index] &lt;- 6446.18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2020</v>
       </c>
@@ -1525,11 +1696,19 @@
         <v>33</v>
       </c>
       <c r="M20" t="str">
-        <f>"y$set$"&amp;G20&amp;"[y$set$set.number == "&amp;C20&amp;"] &lt;- "&amp;I20</f>
+        <f t="shared" si="0"/>
         <v>y$set$latitude.stop[y$set$set.number == 41] &lt;- 4700.13</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N20" t="str">
+        <f t="shared" si="1"/>
+        <v>index = y$set$set.number == 41 PAR y$set$latitude.stop[index] &lt;- 4700.13</v>
+      </c>
+      <c r="O20" t="str">
+        <f t="shared" si="2"/>
+        <v>y$set$latitude.stop[index] &lt;- 4700.13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2020</v>
       </c>
@@ -1559,11 +1738,19 @@
         <v>31</v>
       </c>
       <c r="M21" t="str">
-        <f>"y$set$"&amp;G21&amp;"[y$set$set.number == "&amp;C21&amp;"] &lt;- "&amp;I21</f>
+        <f t="shared" si="0"/>
         <v>y$set$depth.start[y$set$set.number == 43] &lt;- 36</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N21" t="str">
+        <f t="shared" si="1"/>
+        <v>index = y$set$set.number == 43 PAR y$set$depth.start[index] &lt;- 36</v>
+      </c>
+      <c r="O21" t="str">
+        <f t="shared" si="2"/>
+        <v>y$set$depth.start[index] &lt;- 36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2020</v>
       </c>
@@ -1595,11 +1782,19 @@
         <v>31</v>
       </c>
       <c r="M22" t="str">
-        <f>"y$set$"&amp;G22&amp;"[y$set$set.number == "&amp;C22&amp;"] &lt;- "&amp;I22</f>
+        <f t="shared" si="0"/>
         <v>y$set$longitude.start[y$set$set.number == 48] &lt;- 6429.3</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N22" t="str">
+        <f t="shared" si="1"/>
+        <v>index = y$set$set.number == 48 PAR y$set$longitude.start[index] &lt;- 6429.3</v>
+      </c>
+      <c r="O22" t="str">
+        <f t="shared" si="2"/>
+        <v>y$set$longitude.start[index] &lt;- 6429.3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2020</v>
       </c>
@@ -1631,11 +1826,19 @@
         <v>30</v>
       </c>
       <c r="M23" t="str">
-        <f>"y$set$"&amp;G23&amp;"[y$set$set.number == "&amp;C23&amp;"] &lt;- "&amp;I23</f>
+        <f t="shared" si="0"/>
         <v>y$set$depth.end[y$set$set.number == 51] &lt;- 10</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N23" t="str">
+        <f t="shared" si="1"/>
+        <v>index = y$set$set.number == 51 PAR y$set$depth.end[index] &lt;- 10</v>
+      </c>
+      <c r="O23" t="str">
+        <f t="shared" si="2"/>
+        <v>y$set$depth.end[index] &lt;- 10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2020</v>
       </c>
@@ -1667,11 +1870,19 @@
         <v>30</v>
       </c>
       <c r="M24" t="str">
-        <f>"y$set$"&amp;G24&amp;"[y$set$set.number == "&amp;C24&amp;"] &lt;- "&amp;I24</f>
+        <f t="shared" si="0"/>
         <v>y$set$depth.start[y$set$set.number == 53] &lt;- 16</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N24" t="str">
+        <f t="shared" si="1"/>
+        <v>index = y$set$set.number == 53 PAR y$set$depth.start[index] &lt;- 16</v>
+      </c>
+      <c r="O24" t="str">
+        <f t="shared" si="2"/>
+        <v>y$set$depth.start[index] &lt;- 16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2020</v>
       </c>
@@ -1703,11 +1914,19 @@
         <v>30</v>
       </c>
       <c r="M25" t="str">
-        <f>"y$set$"&amp;G25&amp;"[y$set$set.number == "&amp;C25&amp;"] &lt;- "&amp;I25</f>
+        <f t="shared" si="0"/>
         <v>y$set$depth.end[y$set$set.number == 54] &lt;- 12</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N25" t="str">
+        <f t="shared" si="1"/>
+        <v>index = y$set$set.number == 54 PAR y$set$depth.end[index] &lt;- 12</v>
+      </c>
+      <c r="O25" t="str">
+        <f t="shared" si="2"/>
+        <v>y$set$depth.end[index] &lt;- 12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2020</v>
       </c>
@@ -1739,11 +1958,19 @@
         <v>30</v>
       </c>
       <c r="M26" t="str">
-        <f>"y$set$"&amp;G26&amp;"[y$set$set.number == "&amp;C26&amp;"] &lt;- "&amp;I26</f>
+        <f t="shared" si="0"/>
         <v>y$set$depth.start[y$set$set.number == 55] &lt;- 10</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N26" t="str">
+        <f t="shared" si="1"/>
+        <v>index = y$set$set.number == 55 PAR y$set$depth.start[index] &lt;- 10</v>
+      </c>
+      <c r="O26" t="str">
+        <f t="shared" si="2"/>
+        <v>y$set$depth.start[index] &lt;- 10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2020</v>
       </c>
@@ -1768,18 +1995,26 @@
       <c r="H27" s="3">
         <v>0.48194444444444445</v>
       </c>
-      <c r="I27" s="5">
-        <v>0.48402777777777778</v>
+      <c r="I27" s="16" t="s">
+        <v>74</v>
       </c>
       <c r="J27" t="s">
         <v>31</v>
       </c>
       <c r="M27" t="str">
-        <f>"y$set$"&amp;G27&amp;"[y$set$set.number == "&amp;C27&amp;"] &lt;- "&amp;TEXT(I27,"hh:mm:ss")</f>
-        <v>y$set$start.time[y$set$set.number == 56] &lt;- 11:37:00</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>y$set$start.time[y$set$set.number == 56] &lt;- 11:37:00 AM</v>
+      </c>
+      <c r="N27" t="str">
+        <f t="shared" si="1"/>
+        <v>index = y$set$set.number == 56 PAR y$set$start.time[index] &lt;- 11:37:00 AM</v>
+      </c>
+      <c r="O27" t="str">
+        <f t="shared" si="2"/>
+        <v>y$set$start.time[index] &lt;- 11:37:00 AM</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2020</v>
       </c>
@@ -1801,21 +2036,29 @@
       <c r="G28" t="s">
         <v>15</v>
       </c>
-      <c r="H28" s="7">
+      <c r="H28" s="6">
         <v>33</v>
       </c>
-      <c r="I28" s="6">
+      <c r="I28" s="5">
         <v>32</v>
       </c>
       <c r="J28" t="s">
         <v>30</v>
       </c>
       <c r="M28" t="str">
-        <f>"y$set$"&amp;G28&amp;"[y$set$set.number == "&amp;C28&amp;"] &lt;- "&amp;I28</f>
+        <f t="shared" si="0"/>
         <v>y$set$depth.start[y$set$set.number == 58] &lt;- 32</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N28" t="str">
+        <f t="shared" si="1"/>
+        <v>index = y$set$set.number == 58 PAR y$set$depth.start[index] &lt;- 32</v>
+      </c>
+      <c r="O28" t="str">
+        <f t="shared" si="2"/>
+        <v>y$set$depth.start[index] &lt;- 32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2020</v>
       </c>
@@ -1840,18 +2083,26 @@
       <c r="H29" s="2">
         <v>6328.83</v>
       </c>
-      <c r="I29" s="6">
+      <c r="I29" s="5">
         <v>6428.83</v>
       </c>
       <c r="J29" t="s">
         <v>33</v>
       </c>
       <c r="M29" t="str">
-        <f>"y$set$"&amp;G29&amp;"[y$set$set.number == "&amp;C29&amp;"] &lt;- "&amp;I29</f>
+        <f t="shared" si="0"/>
         <v>y$set$longitude.start[y$set$set.number == 66] &lt;- 6428.83</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N29" t="str">
+        <f t="shared" si="1"/>
+        <v>index = y$set$set.number == 66 PAR y$set$longitude.start[index] &lt;- 6428.83</v>
+      </c>
+      <c r="O29" t="str">
+        <f t="shared" si="2"/>
+        <v>y$set$longitude.start[index] &lt;- 6428.83</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2020</v>
       </c>
@@ -1876,18 +2127,26 @@
       <c r="H30" s="2">
         <v>4433.8100000000004</v>
       </c>
-      <c r="I30" s="6">
+      <c r="I30" s="5">
         <v>4633.8100000000004</v>
       </c>
       <c r="J30" t="s">
         <v>33</v>
       </c>
       <c r="M30" t="str">
-        <f>"y$set$"&amp;G30&amp;"[y$set$set.number == "&amp;C30&amp;"] &lt;- "&amp;I30</f>
+        <f t="shared" si="0"/>
         <v>y$set$latitude.start[y$set$set.number == 67] &lt;- 4633.81</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N30" t="str">
+        <f t="shared" si="1"/>
+        <v>index = y$set$set.number == 67 PAR y$set$latitude.start[index] &lt;- 4633.81</v>
+      </c>
+      <c r="O30" t="str">
+        <f t="shared" si="2"/>
+        <v>y$set$latitude.start[index] &lt;- 4633.81</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2020</v>
       </c>
@@ -1919,11 +2178,19 @@
         <v>31</v>
       </c>
       <c r="M31" t="str">
-        <f>"y$set$"&amp;G31&amp;"[y$set$set.number == "&amp;C31&amp;"] &lt;- "&amp;I31</f>
+        <f t="shared" si="0"/>
         <v>y$set$latitude.stop[y$set$set.number == 68] &lt;- 4617.5</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N31" t="str">
+        <f t="shared" si="1"/>
+        <v>index = y$set$set.number == 68 PAR y$set$latitude.stop[index] &lt;- 4617.5</v>
+      </c>
+      <c r="O31" t="str">
+        <f t="shared" si="2"/>
+        <v>y$set$latitude.stop[index] &lt;- 4617.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2020</v>
       </c>
@@ -1955,11 +2222,19 @@
         <v>11</v>
       </c>
       <c r="M32" t="str">
-        <f>"y$set$"&amp;G32&amp;"[y$set$set.number == "&amp;C32&amp;"] &lt;- "&amp;I32</f>
+        <f t="shared" si="0"/>
         <v>y$set$longitude.stop[y$set$set.number == 73] &lt;- 6408.86</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N32" t="str">
+        <f t="shared" si="1"/>
+        <v>index = y$set$set.number == 73 PAR y$set$longitude.stop[index] &lt;- 6408.86</v>
+      </c>
+      <c r="O32" t="str">
+        <f t="shared" si="2"/>
+        <v>y$set$longitude.stop[index] &lt;- 6408.86</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2020</v>
       </c>
@@ -1991,11 +2266,19 @@
         <v>31</v>
       </c>
       <c r="M33" t="str">
-        <f>"y$set$"&amp;G33&amp;"[y$set$set.number == "&amp;C33&amp;"] &lt;- "&amp;I33</f>
+        <f t="shared" si="0"/>
         <v>y$set$latitude.start[y$set$set.number == 75] &lt;- 4626.3</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N33" t="str">
+        <f t="shared" si="1"/>
+        <v>index = y$set$set.number == 75 PAR y$set$latitude.start[index] &lt;- 4626.3</v>
+      </c>
+      <c r="O33" t="str">
+        <f t="shared" si="2"/>
+        <v>y$set$latitude.start[index] &lt;- 4626.3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2020</v>
       </c>
@@ -2027,11 +2310,19 @@
         <v>31</v>
       </c>
       <c r="M34" t="str">
-        <f>"y$set$"&amp;G34&amp;"[y$set$set.number == "&amp;C34&amp;"] &lt;- "&amp;I34</f>
+        <f t="shared" si="0"/>
         <v>y$set$latitude.start[y$set$set.number == 88] &lt;- 4611.99</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N34" t="str">
+        <f t="shared" si="1"/>
+        <v>index = y$set$set.number == 88 PAR y$set$latitude.start[index] &lt;- 4611.99</v>
+      </c>
+      <c r="O34" t="str">
+        <f t="shared" si="2"/>
+        <v>y$set$latitude.start[index] &lt;- 4611.99</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2020</v>
       </c>
@@ -2063,11 +2354,19 @@
         <v>31</v>
       </c>
       <c r="M35" t="str">
-        <f>"y$set$"&amp;G35&amp;"[y$set$set.number == "&amp;C35&amp;"] &lt;- "&amp;I35</f>
+        <f t="shared" si="0"/>
         <v>y$set$station[y$set$set.number == 89] &lt;- B1</v>
       </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N35" t="str">
+        <f t="shared" si="1"/>
+        <v>index = y$set$set.number == 89 PAR y$set$station[index] &lt;- B1</v>
+      </c>
+      <c r="O35" t="str">
+        <f t="shared" si="2"/>
+        <v>y$set$station[index] &lt;- B1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2020</v>
       </c>
@@ -2099,11 +2398,19 @@
         <v>11</v>
       </c>
       <c r="M36" t="str">
-        <f>"y$set$"&amp;G36&amp;"[y$set$set.number == "&amp;C36&amp;"] &lt;- "&amp;I36</f>
+        <f t="shared" si="0"/>
         <v>y$set$latitude.stop[y$set$set.number == 91] &lt;- 4614.45</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N36" t="str">
+        <f t="shared" si="1"/>
+        <v>index = y$set$set.number == 91 PAR y$set$latitude.stop[index] &lt;- 4614.45</v>
+      </c>
+      <c r="O36" t="str">
+        <f t="shared" si="2"/>
+        <v>y$set$latitude.stop[index] &lt;- 4614.45</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2020</v>
       </c>
@@ -2133,11 +2440,19 @@
         <v>35</v>
       </c>
       <c r="M37" t="str">
-        <f>"y$set$"&amp;G37&amp;"[y$set$set.number == "&amp;C37&amp;"] &lt;- "&amp;I37</f>
+        <f t="shared" si="0"/>
         <v>y$set$comment[y$set$set.number == 96] &lt;- Null - Caught chunk of mud</v>
       </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N37" t="str">
+        <f t="shared" si="1"/>
+        <v>index = y$set$set.number == 96 PAR y$set$comment[index] &lt;- Null - Caught chunk of mud</v>
+      </c>
+      <c r="O37" t="str">
+        <f t="shared" si="2"/>
+        <v>y$set$comment[index] &lt;- Null - Caught chunk of mud</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2020</v>
       </c>
@@ -2169,11 +2484,19 @@
         <v>31</v>
       </c>
       <c r="M38" t="str">
-        <f>"y$set$"&amp;G38&amp;"[y$set$set.number == "&amp;C38&amp;"] &lt;- "&amp;I38</f>
+        <f t="shared" si="0"/>
         <v>y$set$station[y$set$set.number == 102] &lt;- 331</v>
       </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N38" t="str">
+        <f t="shared" si="1"/>
+        <v>index = y$set$set.number == 102 PAR y$set$station[index] &lt;- 331</v>
+      </c>
+      <c r="O38" t="str">
+        <f t="shared" si="2"/>
+        <v>y$set$station[index] &lt;- 331</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2020</v>
       </c>
@@ -2205,43 +2528,51 @@
         <v>31</v>
       </c>
       <c r="M39" t="str">
-        <f>"y$set$"&amp;G39&amp;"[y$set$set.number == "&amp;C39&amp;"] &lt;- "&amp;I39</f>
+        <f t="shared" si="0"/>
         <v>y$set$longitude.stop[y$set$set.number == 104] &lt;- 6400.69</v>
       </c>
-    </row>
-    <row r="40" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="10">
-        <v>2020</v>
-      </c>
-      <c r="B40" s="10">
-        <v>150</v>
-      </c>
-      <c r="C40" s="10">
+      <c r="N39" t="str">
+        <f t="shared" si="1"/>
+        <v>index = y$set$set.number == 104 PAR y$set$longitude.stop[index] &lt;- 6400.69</v>
+      </c>
+      <c r="O39" t="str">
+        <f t="shared" si="2"/>
+        <v>y$set$longitude.stop[index] &lt;- 6400.69</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="9">
+        <v>2020</v>
+      </c>
+      <c r="B40" s="9">
+        <v>150</v>
+      </c>
+      <c r="C40" s="9">
         <v>105</v>
       </c>
-      <c r="D40" s="10">
-        <v>5</v>
-      </c>
-      <c r="E40" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F40" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="G40" s="10" t="s">
+      <c r="D40" s="9">
+        <v>5</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F40" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G40" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="H40" s="11" t="s">
+      <c r="H40" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="I40" s="12" t="s">
+      <c r="I40" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="J40" s="10" t="s">
+      <c r="J40" s="9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2020</v>
       </c>
@@ -2276,8 +2607,17 @@
         <f>"y$set$"&amp;G41&amp;"[y$set$set.number == "&amp;C41&amp;"] &lt;- "&amp;I41</f>
         <v>y$set$depth.end[y$set$set.number == 110] &lt;- 19</v>
       </c>
+      <c r="N41" t="str">
+        <f t="shared" si="1"/>
+        <v>index = y$set$set.number == 110 PAR y$set$depth.end[index] &lt;- 19</v>
+      </c>
+      <c r="O41" t="str">
+        <f t="shared" si="2"/>
+        <v>y$set$depth.end[index] &lt;- 19</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:K41"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -2289,7 +2629,7 @@
   <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="L2" sqref="L2:L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2297,6 +2637,7 @@
     <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="97" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -2363,89 +2704,87 @@
         <v>46</v>
       </c>
       <c r="L2" t="str">
-        <f>"y$basket$"&amp;G2&amp;"[y$basket$set.number == "&amp;C2&amp;"] &lt;- "&amp;I2</f>
-        <v>y$basket$Species[y$basket$set.number == ] &lt;- 611</v>
+        <f>"index = y$set$set.number == "&amp;$C2&amp;" PAR "&amp;"y$basket$"&amp;$G2&amp;"[index] &lt;- "&amp;$I2</f>
+        <v>index = y$set$set.number ==  PAR y$basket$Species[index] &lt;- 611</v>
       </c>
       <c r="Q2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10">
-        <v>2020</v>
-      </c>
-      <c r="B3" s="10">
-        <v>150</v>
-      </c>
-      <c r="C3" s="10">
-        <v>5</v>
-      </c>
-      <c r="D3" s="10">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9">
+        <v>2020</v>
+      </c>
+      <c r="B3" s="9">
+        <v>150</v>
+      </c>
+      <c r="C3" s="9">
+        <v>5</v>
+      </c>
+      <c r="D3" s="9">
         <v>6</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="10" t="s">
+      <c r="F3" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="12" t="s">
+      <c r="H3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="J3" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L3" s="10" t="str">
-        <f t="shared" ref="L3:L11" si="0">"y$set$"&amp;G3&amp;"[y$set$set.number == "&amp;C3&amp;"] &lt;- "&amp;I3</f>
-        <v>y$set$Species[y$set$set.number == 5] &lt;- REMOVE?</v>
-      </c>
-      <c r="Q3" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10">
-        <v>2020</v>
-      </c>
-      <c r="B4" s="10">
-        <v>150</v>
-      </c>
-      <c r="C4" s="10">
+      <c r="L3" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q3" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="9">
+        <v>2020</v>
+      </c>
+      <c r="B4" s="9">
+        <v>150</v>
+      </c>
+      <c r="C4" s="9">
         <v>109</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="9">
         <v>6</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="10" t="s">
+      <c r="F4" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="H4" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="I4" s="12" t="s">
+      <c r="H4" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="J4" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="L4" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>y$set$Species[y$set$set.number == 109] &lt;- REMOVE?</v>
-      </c>
-      <c r="Q4" s="10" t="s">
-        <v>67</v>
+      <c r="L4" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q4" s="9" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -2480,11 +2819,11 @@
         <v>47</v>
       </c>
       <c r="L5" t="str">
-        <f t="shared" si="0"/>
-        <v>y$set$sampled[y$set$set.number == 63] &lt;- N</v>
+        <f>"index = y$set$set.number == "&amp;$C5&amp;" PAR "&amp;"y$basket$"&amp;$G5&amp;"[index] &lt;- "&amp;$I5</f>
+        <v>index = y$set$set.number == 63 PAR y$basket$sampled[index] &lt;- N</v>
       </c>
       <c r="Q5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -2519,128 +2858,125 @@
         <v>48</v>
       </c>
       <c r="L6" t="str">
-        <f t="shared" si="0"/>
-        <v>y$set$sampled[y$set$set.number == 76] &lt;- N</v>
+        <f>"index = y$set$set.number == "&amp;$C6&amp;" PAR "&amp;"y$basket$"&amp;$G6&amp;"[index] &lt;- "&amp;$I6</f>
+        <v>index = y$set$set.number == 76 PAR y$basket$sampled[index] &lt;- N</v>
       </c>
       <c r="Q6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="10">
-        <v>2020</v>
-      </c>
-      <c r="B7" s="10">
-        <v>150</v>
-      </c>
-      <c r="C7" s="10">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <v>2020</v>
+      </c>
+      <c r="B7" s="9">
+        <v>150</v>
+      </c>
+      <c r="C7" s="9">
         <v>47</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="9">
         <v>6</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="9">
         <v>63</v>
       </c>
-      <c r="F7" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="10" t="s">
+      <c r="F7" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="H7" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="I7" s="12" t="s">
+      <c r="H7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="J7" s="10" t="s">
+      <c r="J7" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="L7" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>y$set$sampled[y$set$set.number == 47] &lt;- N</v>
-      </c>
-      <c r="Q7" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="10">
-        <v>2020</v>
-      </c>
-      <c r="B8" s="10">
-        <v>150</v>
-      </c>
-      <c r="C8" s="10">
+      <c r="L7" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q7" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <v>2020</v>
+      </c>
+      <c r="B8" s="9">
+        <v>150</v>
+      </c>
+      <c r="C8" s="9">
         <v>74</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="9">
         <v>6</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="9">
         <v>63</v>
       </c>
-      <c r="F8" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" s="10" t="s">
+      <c r="F8" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="H8" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="I8" s="12" t="s">
+      <c r="H8" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="J8" s="10" t="s">
+      <c r="J8" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="L8" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>y$set$sampled[y$set$set.number == 74] &lt;- N</v>
-      </c>
-      <c r="Q8" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="10">
-        <v>2020</v>
-      </c>
-      <c r="B9" s="10">
-        <v>150</v>
-      </c>
-      <c r="C9" s="13">
+      <c r="L8" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q8" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
+        <v>2020</v>
+      </c>
+      <c r="B9" s="9">
+        <v>150</v>
+      </c>
+      <c r="C9" s="12">
         <v>102</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="9">
         <v>6</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="9">
         <v>60</v>
       </c>
-      <c r="F9" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" s="10" t="s">
+      <c r="F9" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="H9" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="I9" s="12" t="s">
+      <c r="H9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="J9" s="10" t="s">
+      <c r="J9" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="L9" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>y$set$sampled[y$set$set.number == 102] &lt;- N</v>
-      </c>
-      <c r="Q9" s="10" t="s">
-        <v>67</v>
+      <c r="L9" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q9" s="9" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -2650,7 +2986,7 @@
       <c r="B10">
         <v>150</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="7">
         <v>57</v>
       </c>
       <c r="D10">
@@ -2675,11 +3011,11 @@
         <v>44</v>
       </c>
       <c r="L10" t="str">
-        <f t="shared" si="0"/>
-        <v>y$set$size.class[y$set$set.number == 57] &lt;- 1</v>
+        <f>"index = y$set$set.number == "&amp;$C10&amp;" PAR "&amp;"y$basket$"&amp;$G10&amp;"[index] &lt;- "&amp;$I10</f>
+        <v>index = y$set$set.number == 57 PAR y$basket$size.class[index] &lt;- 1</v>
       </c>
       <c r="Q10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -2689,13 +3025,13 @@
       <c r="B11">
         <v>150</v>
       </c>
-      <c r="C11" s="8">
-        <v>5</v>
-      </c>
-      <c r="D11" s="8">
+      <c r="C11" s="7">
+        <v>5</v>
+      </c>
+      <c r="D11" s="7">
         <v>6</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11" s="7">
         <v>2539</v>
       </c>
       <c r="F11" t="s">
@@ -2714,11 +3050,11 @@
         <v>45</v>
       </c>
       <c r="L11" t="str">
-        <f t="shared" si="0"/>
-        <v>y$set$sampled[y$set$set.number == 5] &lt;- Y</v>
+        <f>"index = y$set$set.number == "&amp;$C11&amp;" PAR "&amp;"y$basket$"&amp;$G11&amp;"[index] &lt;- "&amp;$I11</f>
+        <v>index = y$set$set.number == 5 PAR y$basket$sampled[index] &lt;- Y</v>
       </c>
       <c r="Q11" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -2730,10 +3066,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q17"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2745,7 +3081,7 @@
     <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -2780,511 +3116,527 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10">
-        <v>2020</v>
-      </c>
-      <c r="B2" s="10">
-        <v>150</v>
-      </c>
-      <c r="C2" s="10">
+    <row r="2" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="13">
+        <v>2020</v>
+      </c>
+      <c r="B2" s="13">
+        <v>150</v>
+      </c>
+      <c r="C2" s="13">
         <v>66</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D2" s="13">
         <v>8</v>
       </c>
-      <c r="E2" s="10">
+      <c r="E2" s="13">
         <v>43</v>
       </c>
-      <c r="F2" s="10">
+      <c r="F2" s="13">
         <v>21733</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="H2" s="11">
+      <c r="H2" s="14">
         <v>1</v>
       </c>
-      <c r="I2" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" s="10" t="s">
+      <c r="I2" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="L2" s="10" t="str">
+      <c r="L2" s="13" t="str">
         <f>"y$bio$"&amp;G2&amp;"[y$bio$set.number == "&amp;C2&amp;"] &lt;- "&amp;I2</f>
         <v>y$bio$length[y$bio$set.number == 66] &lt;- NA</v>
       </c>
-      <c r="Q2" s="10" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10">
-        <v>2020</v>
-      </c>
-      <c r="B3" s="10">
-        <v>150</v>
-      </c>
-      <c r="C3" s="10">
+      <c r="M2" t="str">
+        <f>"index = y$bio$set.number == "&amp;$C2&amp;" AND y$bio$Specimen == "&amp;$F2&amp;" PAR y$bio$"&amp;$G2&amp;"[index] &lt;- "&amp;$I2</f>
+        <v>index = y$bio$set.number == 66 AND y$bio$Specimen == 21733 PAR y$bio$length[index] &lt;- NA</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="13">
+        <v>2020</v>
+      </c>
+      <c r="B3" s="13">
+        <v>150</v>
+      </c>
+      <c r="C3" s="13">
         <v>87</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="13">
         <v>8</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="13">
         <v>43</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="13">
         <v>32083</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="H3" s="11">
+      <c r="H3" s="14">
         <v>1</v>
       </c>
-      <c r="I3" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="J3" s="10" t="s">
+      <c r="I3" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="L3" s="10" t="str">
+      <c r="L3" s="13" t="str">
         <f t="shared" ref="L3:L15" si="0">"y$bio$"&amp;G3&amp;"[y$bio$set.number == "&amp;C3&amp;"] &lt;- "&amp;I3</f>
         <v>y$bio$length[y$bio$set.number == 87] &lt;- NA</v>
       </c>
-      <c r="Q3" s="10" t="s">
+      <c r="M3" t="str">
+        <f t="shared" ref="M3:M15" si="1">"index = y$bio$set.number == "&amp;$C3&amp;" AND y$bio$Specimen == "&amp;$F3&amp;" PAR y$bio$"&amp;$G3&amp;"[index] &lt;- "&amp;$I3</f>
+        <v>index = y$bio$set.number == 87 AND y$bio$Specimen == 32083 PAR y$bio$length[index] &lt;- NA</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="13">
+        <v>2020</v>
+      </c>
+      <c r="B4" s="13">
+        <v>150</v>
+      </c>
+      <c r="C4" s="13">
+        <v>83</v>
+      </c>
+      <c r="D4" s="13">
+        <v>8</v>
+      </c>
+      <c r="E4" s="13">
+        <v>60</v>
+      </c>
+      <c r="F4" s="13">
+        <v>30070</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="H4" s="14">
+        <v>1</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="L4" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>y$bio$length[y$bio$set.number == 83] &lt;- NA</v>
+      </c>
+      <c r="M4" t="str">
+        <f t="shared" si="1"/>
+        <v>index = y$bio$set.number == 83 AND y$bio$Specimen == 30070 PAR y$bio$length[index] &lt;- NA</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="13">
+        <v>2020</v>
+      </c>
+      <c r="B5" s="13">
+        <v>150</v>
+      </c>
+      <c r="C5" s="13">
+        <v>35</v>
+      </c>
+      <c r="D5" s="13">
+        <v>8</v>
+      </c>
+      <c r="E5" s="13">
         <v>63</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10">
-        <v>2020</v>
-      </c>
-      <c r="B4" s="10">
-        <v>150</v>
-      </c>
-      <c r="C4" s="10">
-        <v>83</v>
-      </c>
-      <c r="D4" s="10">
+      <c r="F5" s="13">
+        <v>14057</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="H5" s="14">
+        <v>1</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="L5" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>y$bio$length[y$bio$set.number == 35] &lt;- NA</v>
+      </c>
+      <c r="M5" t="str">
+        <f t="shared" si="1"/>
+        <v>index = y$bio$set.number == 35 AND y$bio$Specimen == 14057 PAR y$bio$length[index] &lt;- NA</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="13">
+        <v>2020</v>
+      </c>
+      <c r="B6" s="13">
+        <v>150</v>
+      </c>
+      <c r="C6" s="13">
+        <v>35</v>
+      </c>
+      <c r="D6" s="13">
         <v>8</v>
       </c>
-      <c r="E4" s="10">
-        <v>60</v>
-      </c>
-      <c r="F4" s="10">
-        <v>30070</v>
-      </c>
-      <c r="G4" s="10" t="s">
+      <c r="E6" s="13">
+        <v>63</v>
+      </c>
+      <c r="F6" s="13">
+        <v>13878</v>
+      </c>
+      <c r="G6" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="H4" s="11">
+      <c r="H6" s="14">
         <v>1</v>
       </c>
-      <c r="I4" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="J4" s="10" t="s">
+      <c r="I6" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="L4" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>y$bio$length[y$bio$set.number == 83] &lt;- NA</v>
-      </c>
-      <c r="Q4" s="10" t="s">
+      <c r="L6" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>y$bio$length[y$bio$set.number == 35] &lt;- NA</v>
+      </c>
+      <c r="M6" t="str">
+        <f t="shared" si="1"/>
+        <v>index = y$bio$set.number == 35 AND y$bio$Specimen == 13878 PAR y$bio$length[index] &lt;- NA</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="13">
+        <v>2020</v>
+      </c>
+      <c r="B7" s="13">
+        <v>150</v>
+      </c>
+      <c r="C7" s="13">
+        <v>70</v>
+      </c>
+      <c r="D7" s="13">
+        <v>8</v>
+      </c>
+      <c r="E7" s="13">
         <v>63</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="10">
-        <v>2020</v>
-      </c>
-      <c r="B5" s="10">
-        <v>150</v>
-      </c>
-      <c r="C5" s="10">
-        <v>35</v>
-      </c>
-      <c r="D5" s="10">
+      <c r="F7" s="13">
+        <v>24129</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="H7" s="14">
+        <v>3</v>
+      </c>
+      <c r="I7" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="J7" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="L7" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>y$bio$length[y$bio$set.number == 70] &lt;- NA</v>
+      </c>
+      <c r="M7" t="str">
+        <f t="shared" si="1"/>
+        <v>index = y$bio$set.number == 70 AND y$bio$Specimen == 24129 PAR y$bio$length[index] &lt;- NA</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="13">
+        <v>2020</v>
+      </c>
+      <c r="B8" s="13">
+        <v>150</v>
+      </c>
+      <c r="C8" s="13">
+        <v>49</v>
+      </c>
+      <c r="D8" s="13">
         <v>8</v>
       </c>
-      <c r="E5" s="10">
-        <v>63</v>
-      </c>
-      <c r="F5" s="10">
-        <v>14057</v>
-      </c>
-      <c r="G5" s="10" t="s">
+      <c r="E8" s="13">
+        <v>2550</v>
+      </c>
+      <c r="F8" s="13">
+        <v>18389</v>
+      </c>
+      <c r="G8" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="H5" s="11">
+      <c r="H8" s="14">
+        <v>0</v>
+      </c>
+      <c r="I8" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="J8" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="L8" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>y$bio$length[y$bio$set.number == 49] &lt;- NA</v>
+      </c>
+      <c r="M8" t="str">
+        <f t="shared" si="1"/>
+        <v>index = y$bio$set.number == 49 AND y$bio$Specimen == 18389 PAR y$bio$length[index] &lt;- NA</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="13">
+        <v>2020</v>
+      </c>
+      <c r="B9" s="13">
+        <v>150</v>
+      </c>
+      <c r="C9" s="13">
+        <v>68</v>
+      </c>
+      <c r="D9" s="13">
+        <v>8</v>
+      </c>
+      <c r="E9" s="13">
+        <v>2550</v>
+      </c>
+      <c r="F9" s="13">
+        <v>22641</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="H9" s="14">
+        <v>2</v>
+      </c>
+      <c r="I9" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="J9" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="L9" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>y$bio$length[y$bio$set.number == 68] &lt;- NA</v>
+      </c>
+      <c r="M9" t="str">
+        <f t="shared" si="1"/>
+        <v>index = y$bio$set.number == 68 AND y$bio$Specimen == 22641 PAR y$bio$length[index] &lt;- NA</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="13">
+        <v>2020</v>
+      </c>
+      <c r="B10" s="13">
+        <v>150</v>
+      </c>
+      <c r="C10" s="13">
+        <v>70</v>
+      </c>
+      <c r="D10" s="13">
+        <v>8</v>
+      </c>
+      <c r="E10" s="13">
+        <v>2550</v>
+      </c>
+      <c r="F10" s="13">
+        <v>23868</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="H10" s="14">
+        <v>0</v>
+      </c>
+      <c r="I10" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="J10" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="L10" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>y$bio$length[y$bio$set.number == 70] &lt;- NA</v>
+      </c>
+      <c r="M10" t="str">
+        <f t="shared" si="1"/>
+        <v>index = y$bio$set.number == 70 AND y$bio$Specimen == 23868 PAR y$bio$length[index] &lt;- NA</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="13">
+        <v>2020</v>
+      </c>
+      <c r="B11" s="13">
+        <v>150</v>
+      </c>
+      <c r="C11" s="13">
+        <v>52</v>
+      </c>
+      <c r="D11" s="13">
+        <v>8</v>
+      </c>
+      <c r="E11" s="13">
+        <v>2550</v>
+      </c>
+      <c r="F11" s="13">
+        <v>18798</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="H11" s="14">
+        <v>6</v>
+      </c>
+      <c r="I11" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="J11" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="L11" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>y$bio$length[y$bio$set.number == 52] &lt;- NA</v>
+      </c>
+      <c r="M11" t="str">
+        <f t="shared" si="1"/>
+        <v>index = y$bio$set.number == 52 AND y$bio$Specimen == 18798 PAR y$bio$length[index] &lt;- NA</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="13">
+        <v>2020</v>
+      </c>
+      <c r="B12" s="13">
+        <v>150</v>
+      </c>
+      <c r="C12" s="13">
+        <v>54</v>
+      </c>
+      <c r="D12" s="13">
+        <v>8</v>
+      </c>
+      <c r="E12" s="13">
+        <v>2550</v>
+      </c>
+      <c r="F12" s="13">
+        <v>19197</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="H12" s="14">
+        <v>8</v>
+      </c>
+      <c r="I12" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="J12" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="L12" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>y$bio$length[y$bio$set.number == 54] &lt;- NA</v>
+      </c>
+      <c r="M12" t="str">
+        <f t="shared" si="1"/>
+        <v>index = y$bio$set.number == 54 AND y$bio$Specimen == 19197 PAR y$bio$length[index] &lt;- NA</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="13">
+        <v>2020</v>
+      </c>
+      <c r="B13" s="13">
+        <v>150</v>
+      </c>
+      <c r="C13" s="13">
+        <v>73</v>
+      </c>
+      <c r="D13" s="13">
+        <v>8</v>
+      </c>
+      <c r="E13" s="13">
+        <v>2550</v>
+      </c>
+      <c r="F13" s="13">
+        <v>26240</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="H13" s="14">
+        <v>6</v>
+      </c>
+      <c r="I13" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="J13" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="L13" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>y$bio$length[y$bio$set.number == 73] &lt;- NA</v>
+      </c>
+      <c r="M13" t="str">
+        <f t="shared" si="1"/>
+        <v>index = y$bio$set.number == 73 AND y$bio$Specimen == 26240 PAR y$bio$length[index] &lt;- NA</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="13">
+        <v>2020</v>
+      </c>
+      <c r="B14" s="13">
+        <v>150</v>
+      </c>
+      <c r="C14" s="13">
+        <v>70</v>
+      </c>
+      <c r="D14" s="13">
+        <v>8</v>
+      </c>
+      <c r="E14" s="13">
+        <v>2550</v>
+      </c>
+      <c r="F14" s="13">
+        <v>23991</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="H14" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="I14" s="15">
         <v>1</v>
       </c>
-      <c r="I5" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="J5" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="L5" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>y$bio$length[y$bio$set.number == 35] &lt;- NA</v>
-      </c>
-      <c r="Q5" s="10" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="10">
-        <v>2020</v>
-      </c>
-      <c r="B6" s="10">
-        <v>150</v>
-      </c>
-      <c r="C6" s="10">
-        <v>35</v>
-      </c>
-      <c r="D6" s="10">
-        <v>8</v>
-      </c>
-      <c r="E6" s="10">
-        <v>63</v>
-      </c>
-      <c r="F6" s="10">
-        <v>13878</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="H6" s="11">
-        <v>1</v>
-      </c>
-      <c r="I6" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="J6" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="L6" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>y$bio$length[y$bio$set.number == 35] &lt;- NA</v>
-      </c>
-      <c r="Q6" s="10" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="10">
-        <v>2020</v>
-      </c>
-      <c r="B7" s="10">
-        <v>150</v>
-      </c>
-      <c r="C7" s="10">
-        <v>70</v>
-      </c>
-      <c r="D7" s="10">
-        <v>8</v>
-      </c>
-      <c r="E7" s="10">
-        <v>63</v>
-      </c>
-      <c r="F7" s="10">
-        <v>24129</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="H7" s="11">
-        <v>3</v>
-      </c>
-      <c r="I7" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="J7" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="L7" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>y$bio$length[y$bio$set.number == 70] &lt;- NA</v>
-      </c>
-      <c r="Q7" s="10" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="10">
-        <v>2020</v>
-      </c>
-      <c r="B8" s="10">
-        <v>150</v>
-      </c>
-      <c r="C8" s="10">
-        <v>49</v>
-      </c>
-      <c r="D8" s="10">
-        <v>8</v>
-      </c>
-      <c r="E8" s="10">
-        <v>2550</v>
-      </c>
-      <c r="F8" s="10">
-        <v>18389</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="H8" s="11">
-        <v>0</v>
-      </c>
-      <c r="I8" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="J8" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="L8" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>y$bio$length[y$bio$set.number == 49] &lt;- NA</v>
-      </c>
-      <c r="Q8" s="10" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="10">
-        <v>2020</v>
-      </c>
-      <c r="B9" s="10">
-        <v>150</v>
-      </c>
-      <c r="C9" s="10">
-        <v>68</v>
-      </c>
-      <c r="D9" s="10">
-        <v>8</v>
-      </c>
-      <c r="E9" s="10">
-        <v>2550</v>
-      </c>
-      <c r="F9" s="10">
-        <v>22641</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="H9" s="11">
-        <v>2</v>
-      </c>
-      <c r="I9" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="J9" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="L9" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>y$bio$length[y$bio$set.number == 68] &lt;- NA</v>
-      </c>
-      <c r="Q9" s="10" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="10">
-        <v>2020</v>
-      </c>
-      <c r="B10" s="10">
-        <v>150</v>
-      </c>
-      <c r="C10" s="10">
-        <v>70</v>
-      </c>
-      <c r="D10" s="10">
-        <v>8</v>
-      </c>
-      <c r="E10" s="10">
-        <v>2550</v>
-      </c>
-      <c r="F10" s="10">
-        <v>23868</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="H10" s="11">
-        <v>0</v>
-      </c>
-      <c r="I10" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="J10" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="L10" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>y$bio$length[y$bio$set.number == 70] &lt;- NA</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="10">
-        <v>2020</v>
-      </c>
-      <c r="B11" s="10">
-        <v>150</v>
-      </c>
-      <c r="C11" s="10">
-        <v>52</v>
-      </c>
-      <c r="D11" s="10">
-        <v>8</v>
-      </c>
-      <c r="E11" s="10">
-        <v>2550</v>
-      </c>
-      <c r="F11" s="10">
-        <v>18798</v>
-      </c>
-      <c r="G11" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="H11" s="11">
-        <v>6</v>
-      </c>
-      <c r="I11" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="J11" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="L11" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>y$bio$length[y$bio$set.number == 52] &lt;- NA</v>
-      </c>
-      <c r="Q11" s="10" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="10">
-        <v>2020</v>
-      </c>
-      <c r="B12" s="10">
-        <v>150</v>
-      </c>
-      <c r="C12" s="10">
-        <v>54</v>
-      </c>
-      <c r="D12" s="10">
-        <v>8</v>
-      </c>
-      <c r="E12" s="10">
-        <v>2550</v>
-      </c>
-      <c r="F12" s="10">
-        <v>19197</v>
-      </c>
-      <c r="G12" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="H12" s="11">
-        <v>8</v>
-      </c>
-      <c r="I12" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="J12" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="L12" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>y$bio$length[y$bio$set.number == 54] &lt;- NA</v>
-      </c>
-      <c r="Q12" s="10" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="10">
-        <v>2020</v>
-      </c>
-      <c r="B13" s="10">
-        <v>150</v>
-      </c>
-      <c r="C13" s="10">
-        <v>73</v>
-      </c>
-      <c r="D13" s="10">
-        <v>8</v>
-      </c>
-      <c r="E13" s="10">
-        <v>2550</v>
-      </c>
-      <c r="F13" s="10">
-        <v>26240</v>
-      </c>
-      <c r="G13" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="H13" s="11">
-        <v>6</v>
-      </c>
-      <c r="I13" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="J13" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="L13" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>y$bio$length[y$bio$set.number == 73] &lt;- NA</v>
-      </c>
-      <c r="Q13" s="10" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="10">
-        <v>2020</v>
-      </c>
-      <c r="B14" s="10">
-        <v>150</v>
-      </c>
-      <c r="C14" s="10">
-        <v>70</v>
-      </c>
-      <c r="D14" s="10">
-        <v>8</v>
-      </c>
-      <c r="E14" s="10">
-        <v>2550</v>
-      </c>
-      <c r="F14" s="10">
-        <v>23991</v>
-      </c>
-      <c r="G14" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="H14" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="I14" s="12">
-        <v>1</v>
-      </c>
-      <c r="J14" s="10" t="s">
+      <c r="J14" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="L14" s="10" t="str">
+      <c r="L14" s="13" t="str">
         <f t="shared" si="0"/>
         <v>y$bio$sex[y$bio$set.number == 70] &lt;- 1</v>
       </c>
-      <c r="Q14" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M14" t="str">
+        <f t="shared" si="1"/>
+        <v>index = y$bio$set.number == 70 AND y$bio$Specimen == 23991 PAR y$bio$sex[index] &lt;- 1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2020</v>
       </c>
@@ -3319,15 +3671,16 @@
         <f t="shared" si="0"/>
         <v>y$bio$egg.condition[y$bio$set.number == 32] &lt;- NA</v>
       </c>
-      <c r="Q15" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
+      <c r="M15" t="str">
+        <f t="shared" si="1"/>
+        <v>index = y$bio$set.number == 32 AND y$bio$Specimen == 12016 PAR y$bio$egg.condition[index] &lt;- NA</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="8"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
+      <c r="A17" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3341,7 +3694,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="J2" sqref="J2:J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3395,16 +3748,16 @@
         <v>2550</v>
       </c>
       <c r="G2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="J2" t="s">
         <v>68</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="J2" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -3421,16 +3774,16 @@
         <v>2550</v>
       </c>
       <c r="G3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H3" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="J3" t="s">
         <v>69</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="J3" t="s">
-        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>